<commit_message>
cambio de de debut sexual y nombres de ejes en español
</commit_message>
<xml_diff>
--- a/SEROFOI/summary_models/BRA-017-01_HPV16.xlsx
+++ b/SEROFOI/summary_models/BRA-017-01_HPV16.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caj_d\OneDrive\Escritorio\Proyecto Fuerza de infección VPH\GIT\hpv_seroprevalence\SEROFOI\summary_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD5D049-806C-41FE-B3BD-61340434D9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4FBDFD-D841-4F2C-972E-7E931FD0E70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,10 +85,10 @@
     <t>Convergencia</t>
   </si>
   <si>
-    <t>Tasa de serorreversion</t>
-  </si>
-  <si>
-    <t>Tasa de serorreversión Rhat</t>
+    <t>Tasa de seroreversion</t>
+  </si>
+  <si>
+    <t>Tasa de seroreversión Rhat</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G8"/>
+      <selection activeCell="A8" sqref="A8:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>